<commit_message>
made a minor change to see how tortoisegit handles diffs with MS Office files
</commit_message>
<xml_diff>
--- a/OtherFiles/Copy-Oil Change Schedule.xlsx
+++ b/OtherFiles/Copy-Oil Change Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimClayton\OneDrive\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimClayton\Desktop\git\Udemy-Git\OtherFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_6794195CBD3B745CD7552B7E10AA0A41FFEE531B" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{C1FB1546-BF32-4FAB-89E1-0429DDEE3A4F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57291BC1-BE93-45A7-9CFD-696AB9E89298}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="20475" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Car</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>235/65R18</t>
+  </si>
+  <si>
+    <t>Never</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,7 +320,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -331,6 +340,9 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -649,7 +661,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +709,9 @@
       <c r="A2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" s="11" t="s">
         <v>18</v>
       </c>
@@ -771,8 +785,8 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated cells b2 and d2
</commit_message>
<xml_diff>
--- a/OtherFiles/Copy-Oil Change Schedule.xlsx
+++ b/OtherFiles/Copy-Oil Change Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimClayton\Desktop\git\Udemy-Git\OtherFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57291BC1-BE93-45A7-9CFD-696AB9E89298}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BA02C4-CD57-487D-A904-7A5317ED5D1D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="20475" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Car</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Never</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -226,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,12 +269,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,7 +317,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -340,7 +337,10 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -661,7 +661,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,9 @@
       <c r="C2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="5">
         <v>43377</v>
       </c>

</xml_diff>